<commit_message>
Added a Feature file for 5 set games Added steps for IMG and BR 5 set games in Tennis.java Added a new Comp Id for IMG 5 set games Added new Excel sheets for all the 5 set games
</commit_message>
<xml_diff>
--- a/att/src/main/resources/incidents/Tennis/TennisAbandonSet2.xlsx
+++ b/att/src/main/resources/incidents/Tennis/TennisAbandonSet2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pelumalai\sportsbookautomation\src\main\resources\incidents\Tennis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgurjar\IdeaProjects\cucumberautomation\att\src\main\resources\incidents\Tennis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDDC4C9-BEA5-4FD0-9798-B7C1CE67AAE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="set1" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="62">
   <si>
     <t>matchTime</t>
   </si>
@@ -206,9 +207,6 @@
   </si>
   <si>
     <t>6,0,0</t>
-  </si>
-  <si>
-    <t>6,1,0</t>
   </si>
   <si>
     <t>0:00:00</t>
@@ -220,7 +218,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -545,26 +543,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125"/>
-    <col min="2" max="2" width="10.7109375"/>
-    <col min="3" max="3" width="13.7109375"/>
-    <col min="4" max="4" width="14.85546875"/>
-    <col min="5" max="5" width="13.42578125"/>
+    <col min="1" max="1" width="15.54296875"/>
+    <col min="2" max="2" width="10.7265625"/>
+    <col min="3" max="3" width="13.7265625"/>
+    <col min="4" max="4" width="14.81640625"/>
+    <col min="5" max="5" width="13.453125"/>
     <col min="6" max="6" width="11"/>
-    <col min="7" max="7" width="10.85546875"/>
-    <col min="8" max="1025" width="8.5703125"/>
+    <col min="7" max="7" width="10.81640625"/>
+    <col min="8" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,9 +591,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -604,9 +602,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -622,7 +620,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -651,7 +649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -680,7 +678,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -709,7 +707,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -738,7 +736,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
         <v>12</v>
       </c>
@@ -752,7 +750,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -781,7 +779,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -810,7 +808,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -839,7 +837,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -868,7 +866,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>12</v>
       </c>
@@ -882,7 +880,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -911,7 +909,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>27</v>
       </c>
@@ -940,7 +938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>38</v>
       </c>
@@ -969,7 +967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>39</v>
       </c>
@@ -998,7 +996,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
         <v>12</v>
       </c>
@@ -1012,7 +1010,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>40</v>
       </c>
@@ -1041,7 +1039,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
@@ -1070,7 +1068,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>42</v>
       </c>
@@ -1099,7 +1097,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>43</v>
       </c>
@@ -1128,7 +1126,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D23" t="s">
         <v>12</v>
       </c>
@@ -1142,7 +1140,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>44</v>
       </c>
@@ -1171,7 +1169,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>45</v>
       </c>
@@ -1200,7 +1198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>46</v>
       </c>
@@ -1229,7 +1227,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>47</v>
       </c>
@@ -1258,7 +1256,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D28" t="s">
         <v>12</v>
       </c>
@@ -1272,7 +1270,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>48</v>
       </c>
@@ -1301,7 +1299,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>49</v>
       </c>
@@ -1330,7 +1328,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>50</v>
       </c>
@@ -1359,7 +1357,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>51</v>
       </c>
@@ -1388,10 +1386,10 @@
         <v>21</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D33" t="s">
         <v>12</v>
       </c>
@@ -1405,7 +1403,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>52</v>
       </c>
@@ -1434,7 +1432,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>53</v>
       </c>
@@ -1463,18 +1461,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E36" t="s">
         <v>59</v>
@@ -1489,35 +1487,6 @@
         <v>1</v>
       </c>
       <c r="I36" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B37" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" t="s">
-        <v>28</v>
-      </c>
-      <c r="E37" t="s">
-        <v>60</v>
-      </c>
-      <c r="F37" t="s">
-        <v>36</v>
-      </c>
-      <c r="G37">
-        <v>2</v>
-      </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
-      <c r="I37" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1528,20 +1497,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.140625"/>
-    <col min="2" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="17.1796875"/>
+    <col min="2" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1552,7 +1521,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1563,7 +1532,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1574,7 +1543,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1585,7 +1554,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1596,7 +1565,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1607,7 +1576,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1618,7 +1587,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1636,14 +1605,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125"/>
+    <col min="1" max="1025" width="8.54296875"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>